<commit_message>
Added sheets for Seqtype-specific labels and Acq-specific labels
</commit_message>
<xml_diff>
--- a/RePronim_Naming_Convention.xlsx
+++ b/RePronim_Naming_Convention.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Dropbox/BBL/BIDS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark3\Documents\PENN_ReproIn\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD16FC9-EBC3-4AA4-8E2A-4179824A9BA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="680" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="1300" yWindow="650" windowWidth="19760" windowHeight="12690" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReProin Naming" sheetId="1" r:id="rId1"/>
     <sheet name="LookUpTable" sheetId="2" r:id="rId2"/>
+    <sheet name="Seqtype-labels" sheetId="3" r:id="rId3"/>
+    <sheet name="ACQ-labels" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="190">
   <si>
     <t>ReProin Name</t>
   </si>
@@ -487,13 +496,124 @@
   </si>
   <si>
     <t>_seq-pcasl-2d-gre</t>
+  </si>
+  <si>
+    <t>-navsetter-T1w</t>
+  </si>
+  <si>
+    <t>-navsetter-T2w</t>
+  </si>
+  <si>
+    <t>-localizer</t>
+  </si>
+  <si>
+    <t>-TOF</t>
+  </si>
+  <si>
+    <t>-AAscout</t>
+  </si>
+  <si>
+    <t>-navsetter</t>
+  </si>
+  <si>
+    <t>-perf</t>
+  </si>
+  <si>
+    <t>-DTI</t>
+  </si>
+  <si>
+    <t>-HARDI</t>
+  </si>
+  <si>
+    <t>-TRACE</t>
+  </si>
+  <si>
+    <t>-DSI</t>
+  </si>
+  <si>
+    <t>-NODDI</t>
+  </si>
+  <si>
+    <t>-B1</t>
+  </si>
+  <si>
+    <t>spec</t>
+  </si>
+  <si>
+    <t>-SVS</t>
+  </si>
+  <si>
+    <t>-CSI</t>
+  </si>
+  <si>
+    <t>-FLAIR</t>
+  </si>
+  <si>
+    <t>-aligned</t>
+  </si>
+  <si>
+    <t>-BC</t>
+  </si>
+  <si>
+    <t>-headcoil</t>
+  </si>
+  <si>
+    <t>-bodycoil</t>
+  </si>
+  <si>
+    <t>-vnavBC</t>
+  </si>
+  <si>
+    <t>-vnavHC</t>
+  </si>
+  <si>
+    <t>-dwi</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>anat-T1w_acq-vNavBC</t>
+  </si>
+  <si>
+    <t>anat-T1w_acq-vNavHC</t>
+  </si>
+  <si>
+    <t>anat-T2w_acq-FLAIR</t>
+  </si>
+  <si>
+    <t>anat-localizer_acq-aligned</t>
+  </si>
+  <si>
+    <t>anat-t2star_acq-qsm</t>
+  </si>
+  <si>
+    <t>anat-vnavsetter_acq-T1w</t>
+  </si>
+  <si>
+    <t>anat-vnavsetter_acq-T2w</t>
+  </si>
+  <si>
+    <t>anat-vnavsetter_acq-BC</t>
+  </si>
+  <si>
+    <t>anat-vnavsetter_acq-headcoil</t>
+  </si>
+  <si>
+    <t>-fmri</t>
+  </si>
+  <si>
+    <t>fmap-EPIdist_acq-fmri</t>
+  </si>
+  <si>
+    <t>fmap-EPIdist_acq-dwi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -568,6 +688,37 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -591,7 +742,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -609,6 +760,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -620,6 +779,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -887,14 +1049,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
@@ -909,7 +1071,7 @@
     <col min="14" max="14" width="106.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>139</v>
       </c>
@@ -947,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -969,7 +1131,7 @@
         <v>anat-scout_ses-01__localizer</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -989,7 +1151,7 @@
         <v>anat-T1w__MPRAGE_TI1100_ipat2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1012,7 +1174,7 @@
         <v>func-asl_acq-pCASL__ep2d_se_pcasl_PHC_1200ms</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1035,7 +1197,7 @@
         <v>func-bold-singlerep_acq-singleRep__epi_singlerep_advshim</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1055,7 +1217,7 @@
         <v>fmap-onesize__B0map_onesizefitsall_v3</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1078,7 +1240,7 @@
         <v>func-bold_task-fractalNback__bbl1_frac2back1_231</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1101,7 +1263,7 @@
         <v>func-bold_task-EmoID__bbl1_idemo2_210</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1127,7 +1289,7 @@
         <v>dwi-singleshell_acq-35vol_dir-AP__DTI_2x32_35</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1153,7 +1315,7 @@
         <v>dwi-singleshell_acq-36vol_dir-AP__DTI_2x32_36</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="5" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1179,7 +1341,7 @@
         <v>func-rest_task-restbold_acq-124volume__bbl1_restbold1_124</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>138</v>
       </c>
@@ -1219,7 +1381,7 @@
         <v>[PREFIX:] &lt;seqtype[-label]&gt;_ses-&lt;SESID&gt;_task-&lt;TASKID&gt;_acq-&lt;ACQLABEL&gt;_run-&lt;RUNID&gt;_dir-[AP,PA,LR,RL,VD,DV]&lt;more BIDS&gt;__Motive</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15" s="15" t="s">
         <v>109</v>
       </c>
@@ -1241,7 +1403,7 @@
         <v>anatscout_ses-01__localizer_32ch</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" s="16" t="s">
         <v>110</v>
       </c>
@@ -1260,7 +1422,7 @@
         <v>anat-navsetter_T1w__ABCD_T1w_MPR_vNav_setter</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14">
       <c r="A17" s="16" t="s">
         <v>111</v>
       </c>
@@ -1279,7 +1441,7 @@
         <v>anat-T1w__ABCD_T1w_MPR_vNav</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14">
       <c r="A18" s="16" t="s">
         <v>112</v>
       </c>
@@ -1301,7 +1463,7 @@
         <v>fmap_acq-fMRIdistmap_dir-PA__ABCD_fMRI_DistortionMap_PA</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14">
       <c r="A19" s="16" t="s">
         <v>113</v>
       </c>
@@ -1323,7 +1485,7 @@
         <v>fmap_acq-fMRIdistmap_dir-AP__ABCD_fMRI_DistortionMap_AP</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14">
       <c r="A20" s="16" t="s">
         <v>114</v>
       </c>
@@ -1348,7 +1510,7 @@
         <v>func-bold_task-motive1_run-01__ABCD_fMRI_motive1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14">
       <c r="A21" s="16" t="s">
         <v>115</v>
       </c>
@@ -1373,7 +1535,7 @@
         <v>func-bold_task-motive2_run-02__ABCD_fMRI_motive2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14">
       <c r="A22" s="16" t="s">
         <v>116</v>
       </c>
@@ -1398,7 +1560,7 @@
         <v>func-bold_task-motive3_run-03__ABCD_fMRI_motive3</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14">
       <c r="A23" s="16" t="s">
         <v>117</v>
       </c>
@@ -1423,7 +1585,7 @@
         <v>func-bold_task-restbold_run-01__ABCD_fMRI_rest</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14">
       <c r="A24" s="16" t="s">
         <v>117</v>
       </c>
@@ -1448,7 +1610,7 @@
         <v>func-bold_task-restbold_run-02__ABCD_fMRI_rest</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14">
       <c r="A25" s="16" t="s">
         <v>118</v>
       </c>
@@ -1467,37 +1629,37 @@
         <v>anat-qsm__QSM_SWI_1.5mm</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14">
       <c r="A32" s="14" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" s="12" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="12" t="s">
         <v>150</v>
       </c>
@@ -1506,66 +1668,54 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>LookUpTable!$A$2:$A$5</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C13 C15:C27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>LookUpTable!$B$2:$B$200</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D13 D15:D27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>LookUpTable!$C$2:$C$200</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E13 E15:E27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>LookUpTable!$F$2:$F$11</xm:f>
           </x14:formula1>
           <xm:sqref>H2:H13 H15:H27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>LookUpTable!$G$2:$G$7</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I13 I15:I27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>LookUpTable!$H$2:$H$200</xm:f>
           </x14:formula1>
           <xm:sqref>J2:J26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>LookUpTable!$E$2:$E$200</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G13</xm:sqref>
+          <xm:sqref>G2:G13 G15:G27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>LookUpTable!$E$2:$E$200</xm:f>
-          </x14:formula1>
-          <xm:sqref>G15:G27</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
             <xm:f>LookUpTable!$D$2:$D$200</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F13</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>LookUpTable!$D$2:$D$200</xm:f>
-          </x14:formula1>
-          <xm:sqref>F15:F27</xm:sqref>
+          <xm:sqref>F2:F13 F15:F27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1574,21 +1724,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection sqref="A1:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="4" max="4" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1617,7 +1773,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1646,7 +1802,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1675,7 +1831,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1704,7 +1860,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1733,7 +1889,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="B6" s="7" t="s">
         <v>119</v>
       </c>
@@ -1756,7 +1912,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="B7" s="7" t="s">
         <v>120</v>
       </c>
@@ -1779,7 +1935,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="B8" s="7" t="s">
         <v>121</v>
       </c>
@@ -1796,7 +1952,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="B9" s="7" t="s">
         <v>99</v>
       </c>
@@ -1813,7 +1969,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="B10" s="7" t="s">
         <v>122</v>
       </c>
@@ -1830,7 +1986,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="B11" s="7" t="s">
         <v>123</v>
       </c>
@@ -1841,7 +1997,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="B12" s="7" t="s">
         <v>124</v>
       </c>
@@ -1849,7 +2005,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="B13" s="7" t="s">
         <v>125</v>
       </c>
@@ -1857,7 +2013,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="B14" s="7" t="s">
         <v>126</v>
       </c>
@@ -1865,7 +2021,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="B15" s="7" t="s">
         <v>127</v>
       </c>
@@ -1873,7 +2029,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="B16" s="7" t="s">
         <v>128</v>
       </c>
@@ -1881,7 +2037,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15">
       <c r="B17" s="7" t="s">
         <v>129</v>
       </c>
@@ -1889,15 +2045,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15">
       <c r="B18" s="7" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15">
       <c r="B19" s="13" t="s">
         <v>145</v>
       </c>
@@ -1905,7 +2061,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15">
       <c r="B20" s="6" t="s">
         <v>146</v>
       </c>
@@ -1914,92 +2070,95 @@
       </c>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15">
+      <c r="B21" s="7" t="s">
+        <v>154</v>
+      </c>
       <c r="C21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15">
       <c r="C22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15">
       <c r="C23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15">
       <c r="C24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15">
       <c r="C25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15">
       <c r="C26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15">
       <c r="C27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15">
       <c r="C28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15">
       <c r="C29" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15">
       <c r="C30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15">
       <c r="C31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15">
       <c r="C32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:3">
       <c r="C33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:3">
       <c r="C34" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:3">
       <c r="C35" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:3">
       <c r="C36" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:3">
       <c r="C37" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:3">
       <c r="C38" t="s">
         <v>58</v>
       </c>
@@ -2007,4 +2166,364 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0F359C-838D-4A8C-9230-8E484EF9182B}">
+  <dimension ref="A1:N33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetData>
+    <row r="1" spans="1:14" s="17" customFormat="1">
+      <c r="A1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="M2" t="s">
+        <v>166</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="B3" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="B4" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="B5" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="B6" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="B7" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="B8" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="B9" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="B10" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="B11" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="B27" s="13"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" s="7"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N2:N3">
+    <sortCondition ref="N2:N3"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38AA74BC-97FE-424C-80EF-B88742007D8B}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <cols>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35.75" style="20" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" style="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C11">
+    <sortCondition ref="B2:B11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>